<commit_message>
Symulacja oszczednosci na ogrzewaniu z tytułu użytkowania rolet zewnętrznych
</commit_message>
<xml_diff>
--- a/plan/Zestawienie okien.xlsx
+++ b/plan/Zestawienie okien.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
   <si>
     <t>Parter:</t>
   </si>
@@ -118,13 +118,115 @@
   </si>
   <si>
     <t>nad wc</t>
+  </si>
+  <si>
+    <t>Powierzchnia okna [m2]</t>
+  </si>
+  <si>
+    <t>Razem</t>
+  </si>
+  <si>
+    <t>Wspolczynnik U dla okna</t>
+  </si>
+  <si>
+    <t>standardowe okna</t>
+  </si>
+  <si>
+    <t>W/(m2*K)</t>
+  </si>
+  <si>
+    <t>Srednie najniższe temperatury</t>
+  </si>
+  <si>
+    <t>Tempratura w domu</t>
+  </si>
+  <si>
+    <t>Srednie  temperatury</t>
+  </si>
+  <si>
+    <t>Rocznie</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Strata ciepla (okno)</t>
+  </si>
+  <si>
+    <t>Strata ciepła(okno+roleta)</t>
+  </si>
+  <si>
+    <t>okna z roletą</t>
+  </si>
+  <si>
+    <t>oszczedność</t>
+  </si>
+  <si>
+    <t>Różnice temp</t>
+  </si>
+  <si>
+    <t>Godzin w miesiącu zasuniętej rolety</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>strata</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>Koszt 1kWh dla kotła kondensacyjnego</t>
+  </si>
+  <si>
+    <t>zł/rok</t>
+  </si>
+  <si>
+    <t>Cena rolet za m2</t>
+  </si>
+  <si>
+    <t>od</t>
+  </si>
+  <si>
+    <t>Koszt rolet</t>
+  </si>
+  <si>
+    <t>suma</t>
+  </si>
+  <si>
+    <t>godzin</t>
+  </si>
+  <si>
+    <t>cały dzień</t>
+  </si>
+  <si>
+    <t>dzień</t>
+  </si>
+  <si>
+    <t>noc</t>
+  </si>
+  <si>
+    <t>stratakWh/rok</t>
+  </si>
+  <si>
+    <t>Godzin nocnych</t>
+  </si>
+  <si>
+    <t>Godzin zasunietej rolety</t>
+  </si>
+  <si>
+    <t>zasunieta roleta</t>
+  </si>
+  <si>
+    <t>niezasunieta roleta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,16 +235,87 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.35"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA0C8F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC8DCF0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8C00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -150,12 +323,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -450,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J43" sqref="C40:J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -462,21 +810,44 @@
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="15"/>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
@@ -485,15 +856,42 @@
       <c r="E2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="G2">
+        <f>0.9*1.2*2</f>
+        <v>2.16</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="17"/>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="21" t="s">
         <v>27</v>
       </c>
       <c r="D3" t="s">
@@ -502,15 +900,42 @@
       <c r="E3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="G3">
+        <f>0.9*1.5*2</f>
+        <v>2.7</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="17"/>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="21" t="s">
         <v>28</v>
       </c>
       <c r="D4" t="s">
@@ -519,8 +944,29 @@
       <c r="E4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="G4">
+        <f>2.1*1.5</f>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="17"/>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -530,15 +976,44 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="G5">
+        <f>4*2.26</f>
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="H5">
+        <f>3*1300*2260/1000</f>
+        <v>8814</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2">
+        <v>20</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="17"/>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="21" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
@@ -547,15 +1022,37 @@
       <c r="E6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="G6">
+        <v>1.08</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="17"/>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="21" t="s">
         <v>31</v>
       </c>
       <c r="D7" t="s">
@@ -564,15 +1061,62 @@
       <c r="E7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="G7">
+        <f>1.5*1.2</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="4">
+        <v>-0.5</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M7" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="N7" s="7">
+        <v>9.9</v>
+      </c>
+      <c r="O7" s="8">
+        <v>14.9</v>
+      </c>
+      <c r="P7" s="9">
+        <v>18.2</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="R7" s="9">
+        <v>19.5</v>
+      </c>
+      <c r="S7" s="10">
+        <v>15.2</v>
+      </c>
+      <c r="T7" s="7">
+        <v>10</v>
+      </c>
+      <c r="U7" s="6">
+        <v>4.7</v>
+      </c>
+      <c r="V7" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="17"/>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="21" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
@@ -581,15 +1125,76 @@
       <c r="E8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="G8" s="1">
+        <f>1.2*0.6</f>
+        <v>0.72</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="2">
+        <f>$N$5-K7</f>
+        <v>20.5</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" ref="L8:V8" si="0">$N$5-L7</f>
+        <v>19.899999999999999</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="0"/>
+        <v>15.8</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>10.1</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10000000000000142</v>
+      </c>
+      <c r="R8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="U8" s="2">
+        <f t="shared" si="0"/>
+        <v>15.3</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="0"/>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="17"/>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="21" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
@@ -598,15 +1203,78 @@
       <c r="E9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="G9">
+        <v>0.72</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" ref="K9:V9" si="1">$G$11*K8*$M$2</f>
+        <v>498.12950000000001</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="1"/>
+        <v>483.55009999999999</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="1"/>
+        <v>383.92420000000004</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="1"/>
+        <v>245.41989999999998</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>123.92490000000001</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="1"/>
+        <v>43.73820000000002</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="1"/>
+        <v>2.4299000000000346</v>
+      </c>
+      <c r="R9" s="2">
+        <f t="shared" si="1"/>
+        <v>12.149500000000002</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="1"/>
+        <v>116.63520000000003</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="1"/>
+        <v>242.99000000000004</v>
+      </c>
+      <c r="U9" s="2">
+        <f t="shared" si="1"/>
+        <v>371.77470000000005</v>
+      </c>
+      <c r="V9" s="2">
+        <f t="shared" si="1"/>
+        <v>471.40060000000005</v>
+      </c>
+      <c r="W9" s="2">
+        <f>SUM(K9:V9)</f>
+        <v>2996.0666999999999</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="17"/>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="21" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
@@ -615,13 +1283,151 @@
       <c r="E10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="G10">
+        <v>0.72</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" ref="K10:V10" si="2">$G$11*K8*$M$3</f>
+        <v>362.27600000000001</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="2"/>
+        <v>351.6728</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>279.2176</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>178.4872</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="2"/>
+        <v>90.127200000000002</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="2"/>
+        <v>31.809600000000014</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.767200000000025</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="2"/>
+        <v>8.8360000000000003</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="2"/>
+        <v>84.825600000000009</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="2"/>
+        <v>176.72000000000003</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="2"/>
+        <v>270.38160000000005</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="2"/>
+        <v>342.83680000000004</v>
+      </c>
+      <c r="W10" s="2">
+        <f>SUM(K10:V10)</f>
+        <v>2178.9576000000002</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="17"/>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <f>SUM(G2:G10)</f>
+        <v>22.09</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="2">
+        <f>31*12</f>
+        <v>372</v>
+      </c>
+      <c r="L11" s="2">
+        <f>28*12</f>
+        <v>336</v>
+      </c>
+      <c r="M11" s="2">
+        <f>31*10</f>
+        <v>310</v>
+      </c>
+      <c r="N11" s="2">
+        <f>30*8</f>
+        <v>240</v>
+      </c>
+      <c r="O11" s="2">
+        <f>31*8</f>
+        <v>248</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2">
+        <f>30*8</f>
+        <v>240</v>
+      </c>
+      <c r="T11" s="2">
+        <f>30*10</f>
+        <v>300</v>
+      </c>
+      <c r="U11" s="2">
+        <v>310</v>
+      </c>
+      <c r="V11" s="2">
+        <v>372</v>
+      </c>
+      <c r="W11" s="2">
+        <f>SUM(K11:V11)</f>
+        <v>2728</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="17"/>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="16"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="17"/>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -640,8 +1446,32 @@
       <c r="G13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="16"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W13" s="2">
+        <f>W9-W10</f>
+        <v>817.10909999999967</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="17"/>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -657,8 +1487,35 @@
       <c r="G14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="16"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2">
+        <f>W13*W11/1000</f>
+        <v>2229.0736247999989</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y14" s="2">
+        <f>W14*O27</f>
+        <v>468.10546120799978</v>
+      </c>
+      <c r="Z14" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -677,12 +1534,25 @@
       <c r="G15" t="s">
         <v>30</v>
       </c>
-      <c r="I15">
-        <f>865*2095*2/1000000</f>
-        <v>3.6243500000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="16"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="17"/>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -698,8 +1568,27 @@
       <c r="G16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="J16" s="16"/>
+      <c r="K16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="17"/>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -715,8 +1604,49 @@
       <c r="G17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="J17" s="16"/>
+      <c r="K17" s="11">
+        <v>-4</v>
+      </c>
+      <c r="L17" s="4">
+        <v>-3</v>
+      </c>
+      <c r="M17" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="N17" s="12">
+        <v>6.2</v>
+      </c>
+      <c r="O17" s="7">
+        <v>10.3</v>
+      </c>
+      <c r="P17" s="8">
+        <v>14.4</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>15.3</v>
+      </c>
+      <c r="R17" s="10">
+        <v>15.2</v>
+      </c>
+      <c r="S17" s="7">
+        <v>11.2</v>
+      </c>
+      <c r="T17" s="12">
+        <v>6.2</v>
+      </c>
+      <c r="U17" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V17" s="4">
+        <v>-2.4</v>
+      </c>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="17"/>
+    </row>
+    <row r="18" spans="1:27">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -732,8 +1662,70 @@
       <c r="G18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="J18" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="2">
+        <f>$N$5-K17</f>
+        <v>24</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" ref="L18" si="3">$N$5-L17</f>
+        <v>23</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" ref="M18" si="4">$N$5-M17</f>
+        <v>20.3</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" ref="N18" si="5">$N$5-N17</f>
+        <v>13.8</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" ref="O18" si="6">$N$5-O17</f>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" ref="P18" si="7">$N$5-P17</f>
+        <v>5.6</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" ref="Q18" si="8">$N$5-Q17</f>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" ref="R18" si="9">$N$5-R17</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" ref="S18" si="10">$N$5-S17</f>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" ref="T18" si="11">$N$5-T17</f>
+        <v>13.8</v>
+      </c>
+      <c r="U18" s="2">
+        <f t="shared" ref="U18" si="12">$N$5-U17</f>
+        <v>17.7</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" ref="V18" si="13">$N$5-V17</f>
+        <v>22.4</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z18" s="17"/>
+      <c r="AA18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -749,8 +1741,62 @@
       <c r="G19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="J19" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="2">
+        <f>$G$11*K18*$M$2</f>
+        <v>583.17600000000004</v>
+      </c>
+      <c r="L19" s="2">
+        <f>$G$11*L18*$M$2</f>
+        <v>558.87700000000007</v>
+      </c>
+      <c r="M19" s="2">
+        <f>$G$11*M18*$M$2</f>
+        <v>493.26970000000006</v>
+      </c>
+      <c r="N19" s="2">
+        <f>$G$11*N18*$M$2</f>
+        <v>335.32620000000009</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2">
+        <f>$G$11*T18*$M$2</f>
+        <v>335.32620000000009</v>
+      </c>
+      <c r="U19" s="2">
+        <f>$G$11*U18*$M$2</f>
+        <v>430.09230000000002</v>
+      </c>
+      <c r="V19" s="2">
+        <f>$G$11*V18*$M$2</f>
+        <v>544.29759999999999</v>
+      </c>
+      <c r="W19" s="2">
+        <f>SUM(K19:V19)</f>
+        <v>3280.3649999999998</v>
+      </c>
+      <c r="X19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y19" s="2">
+        <f>7*30.5*24</f>
+        <v>5124</v>
+      </c>
+      <c r="Z19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA19">
+        <f>Y19*W19/1000</f>
+        <v>16808.590259999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -763,10 +1809,333 @@
       <c r="G20" t="s">
         <v>30</v>
       </c>
+      <c r="J20" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="2">
+        <f>$G$11*K18*$M$3</f>
+        <v>424.12799999999999</v>
+      </c>
+      <c r="L20" s="2">
+        <f>$G$11*L18*$M$3</f>
+        <v>406.45600000000002</v>
+      </c>
+      <c r="M20" s="2">
+        <f>$G$11*M18*$M$3</f>
+        <v>358.74160000000006</v>
+      </c>
+      <c r="N20" s="2">
+        <f>$G$11*N18*$M$3</f>
+        <v>243.87360000000004</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2">
+        <f>$G$11*T18*$M$3</f>
+        <v>243.87360000000004</v>
+      </c>
+      <c r="U20" s="2">
+        <f>$G$11*U18*$M$3</f>
+        <v>312.7944</v>
+      </c>
+      <c r="V20" s="2">
+        <f>$G$11*V18*$M$3</f>
+        <v>395.8528</v>
+      </c>
+      <c r="W20" s="2">
+        <f>SUM(K20:V20)</f>
+        <v>2385.7200000000003</v>
+      </c>
+      <c r="X20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y20" s="2">
+        <v>5124</v>
+      </c>
+      <c r="Z20" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA20">
+        <f>Y20*W20/1000</f>
+        <v>12224.42928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="J21" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" s="2">
+        <f>31*12</f>
+        <v>372</v>
+      </c>
+      <c r="L21" s="2">
+        <f>28*12</f>
+        <v>336</v>
+      </c>
+      <c r="M21" s="2">
+        <f>31*10</f>
+        <v>310</v>
+      </c>
+      <c r="N21" s="2">
+        <f>30*8</f>
+        <v>240</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2">
+        <f>30*10</f>
+        <v>300</v>
+      </c>
+      <c r="U21" s="2">
+        <f>31*12</f>
+        <v>372</v>
+      </c>
+      <c r="V21" s="2">
+        <f>31*12</f>
+        <v>372</v>
+      </c>
+      <c r="W21" s="2">
+        <f>SUM(K21:V21)</f>
+        <v>2302</v>
+      </c>
+      <c r="X21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="J22" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="2">
+        <f>31*19</f>
+        <v>589</v>
+      </c>
+      <c r="L22" s="2">
+        <f>28*18</f>
+        <v>504</v>
+      </c>
+      <c r="M22" s="2">
+        <f>31*17</f>
+        <v>527</v>
+      </c>
+      <c r="N22" s="2">
+        <f>30*16</f>
+        <v>480</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2">
+        <f>31*17</f>
+        <v>527</v>
+      </c>
+      <c r="U22" s="2">
+        <f>30*18</f>
+        <v>540</v>
+      </c>
+      <c r="V22" s="2">
+        <f>31*19</f>
+        <v>589</v>
+      </c>
+      <c r="W22" s="2">
+        <f>SUM(K22:V22)</f>
+        <v>3756</v>
+      </c>
+      <c r="X22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>3756</v>
+      </c>
+      <c r="Z22" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA22">
+        <f>Y22*W20/1000</f>
+        <v>8960.7643200000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="J23" s="16"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2">
+        <f>Y19-W22</f>
+        <v>1368</v>
+      </c>
+      <c r="X23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>1368</v>
+      </c>
+      <c r="Z23" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA23">
+        <f>Y23*W19/1000</f>
+        <v>4487.539319999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="J24" s="16"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24">
+        <f>AA23+AA22</f>
+        <v>13448.303639999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="J25" s="16"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2">
+        <f>AA19-AA24</f>
+        <v>3360.2866199999989</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y25" s="2">
+        <f>W25*O27</f>
+        <v>705.66019019999976</v>
+      </c>
+      <c r="Z25" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="J26" s="16"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="17"/>
+    </row>
+    <row r="27" spans="1:27">
+      <c r="J27" s="16"/>
+      <c r="K27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="17"/>
+    </row>
+    <row r="28" spans="1:27" ht="15.75" thickBot="1">
+      <c r="J28" s="18"/>
+      <c r="K28" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N28" s="19">
+        <v>180</v>
+      </c>
+      <c r="O28" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="P28" s="19">
+        <f>N28*G11</f>
+        <v>3976.2</v>
+      </c>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="20"/>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
wybór producentow okien, drzwi, bram
</commit_message>
<xml_diff>
--- a/plan/Zestawienie okien.xlsx
+++ b/plan/Zestawienie okien.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="Zestawienie okien" sheetId="1" r:id="rId1"/>
+    <sheet name="Producenci okien" sheetId="2" r:id="rId2"/>
+    <sheet name="Brama garażowa" sheetId="3" r:id="rId3"/>
+    <sheet name="Drzwi wejściowe" sheetId="4" r:id="rId4"/>
+    <sheet name="Okna połaciowe" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="157">
   <si>
     <t>Parter:</t>
   </si>
@@ -220,13 +222,287 @@
   </si>
   <si>
     <t>niezasunieta roleta</t>
+  </si>
+  <si>
+    <t>Producent</t>
+  </si>
+  <si>
+    <t>Drutex</t>
+  </si>
+  <si>
+    <t>PN-PT</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
+  </si>
+  <si>
+    <t>8:00-17:00</t>
+  </si>
+  <si>
+    <t>9:00 – 17:00</t>
+  </si>
+  <si>
+    <t>10:00 – 15:00</t>
+  </si>
+  <si>
+    <t>Oknoplast</t>
+  </si>
+  <si>
+    <t>Vetrex</t>
+  </si>
+  <si>
+    <t>Eurocolor</t>
+  </si>
+  <si>
+    <t>603 034 463</t>
+  </si>
+  <si>
+    <t>Jarosław Strusiński</t>
+  </si>
+  <si>
+    <t>W/m2K</t>
+  </si>
+  <si>
+    <t>Maco</t>
+  </si>
+  <si>
+    <t>do 4</t>
+  </si>
+  <si>
+    <t>okna IGLO ENERGY</t>
+  </si>
+  <si>
+    <t>drzwi Iglo5</t>
+  </si>
+  <si>
+    <t>b.d.</t>
+  </si>
+  <si>
+    <t>brak przesuwnych</t>
+  </si>
+  <si>
+    <t>Winergetic Premium</t>
+  </si>
+  <si>
+    <t>brzydkie</t>
+  </si>
+  <si>
+    <t>drzwi HSK</t>
+  </si>
+  <si>
+    <t>Normstahl</t>
+  </si>
+  <si>
+    <t>Hormann</t>
+  </si>
+  <si>
+    <t>Wiśniowski</t>
+  </si>
+  <si>
+    <t>Gerda</t>
+  </si>
+  <si>
+    <t>Producenci</t>
+  </si>
+  <si>
+    <t>Porta Drzwi</t>
+  </si>
+  <si>
+    <t>Renoma 2000</t>
+  </si>
+  <si>
+    <t>ul. Legnicka 46</t>
+  </si>
+  <si>
+    <t>9:00-18:00</t>
+  </si>
+  <si>
+    <t>Pn-Pt</t>
+  </si>
+  <si>
+    <t>So</t>
+  </si>
+  <si>
+    <t>Przedstawiciel</t>
+  </si>
+  <si>
+    <t>Adres</t>
+  </si>
+  <si>
+    <t>Punkt sprzedaży</t>
+  </si>
+  <si>
+    <t>Godziny otwarcia</t>
+  </si>
+  <si>
+    <t>Ekodynamic Sp. z o.o. Spółka Komandytowa
+ul. Karmelkowa 29 pawilon nr 8</t>
+  </si>
+  <si>
+    <t>ELEKTRYK-SYSTEM NOWOCZESNE TECHNOLOGIE 
+ul. Ładna 17</t>
+  </si>
+  <si>
+    <t>ADOMEX
+ul. Krynicka 1, paw.1a</t>
+  </si>
+  <si>
+    <t>10:00-17:30</t>
+  </si>
+  <si>
+    <t>Wrocław - MIKOŁAJCZYK - Partner Handlowy
+Legnicka 62</t>
+  </si>
+  <si>
+    <t>Fix
+Bystrzycka 69c</t>
+  </si>
+  <si>
+    <t>10:00-18:00 (Pn, Śr)
+9:00-17:00 (Wt, Czw)
+10:00-17:00 (Pt)</t>
+  </si>
+  <si>
+    <t>9:00-13:00 (1 So mies)</t>
+  </si>
+  <si>
+    <t>Krótki przegląd okien</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Komory</t>
+  </si>
+  <si>
+    <t>Okucia</t>
+  </si>
+  <si>
+    <t>Szyby</t>
+  </si>
+  <si>
+    <t>Kolorystyka</t>
+  </si>
+  <si>
+    <t>Uwagi</t>
+  </si>
+  <si>
+    <t>Gwarancja</t>
+  </si>
+  <si>
+    <t>PremiumCenter</t>
+  </si>
+  <si>
+    <t>Kromera 25B</t>
+  </si>
+  <si>
+    <t>kontakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Przedsiębiorstwo MICHALCZYK </t>
+  </si>
+  <si>
+    <t>ul. Kościelna 2 (-&gt;Bielany)</t>
+  </si>
+  <si>
+    <t>8:00-16:00</t>
+  </si>
+  <si>
+    <t>9:00-13:00</t>
+  </si>
+  <si>
+    <t>ul.Fabryczna 6/8</t>
+  </si>
+  <si>
+    <t>Irga, Dzik Józef</t>
+  </si>
+  <si>
+    <t>Fakro</t>
+  </si>
+  <si>
+    <t>Velux</t>
+  </si>
+  <si>
+    <t>PolSkone</t>
+  </si>
+  <si>
+    <t>Nawiewniki</t>
+  </si>
+  <si>
+    <t>Uchylność</t>
+  </si>
+  <si>
+    <t>Parapety</t>
+  </si>
+  <si>
+    <t>Grubość zbrojenia</t>
+  </si>
+  <si>
+    <t>mniej ważne, ważniejsza klasa A,B,C czyli grubość profilu</t>
+  </si>
+  <si>
+    <t>min 1,5mm, często stosują mniejsze; min co 30cm</t>
+  </si>
+  <si>
+    <t>Klamki</t>
+  </si>
+  <si>
+    <t>ile wytrzymują cykli</t>
+  </si>
+  <si>
+    <t>rodzaj, a nie nazwa firmy</t>
+  </si>
+  <si>
+    <t>Izolacja akustyczna</t>
+  </si>
+  <si>
+    <t>Aprobatę techniczną InstytutuTechniki Budowlanej.</t>
+  </si>
+  <si>
+    <t>musi być</t>
+  </si>
+  <si>
+    <t>zakres gwarancji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cena </t>
+  </si>
+  <si>
+    <t>całego okna</t>
+  </si>
+  <si>
+    <t>nazwa/producent</t>
+  </si>
+  <si>
+    <t>ile szyb</t>
+  </si>
+  <si>
+    <t>czy produkują bez</t>
+  </si>
+  <si>
+    <t>czy są do kompletu</t>
+  </si>
+  <si>
+    <t>co jest a co nie jest w nią wliczone</t>
+  </si>
+  <si>
+    <t>Dodatki</t>
+  </si>
+  <si>
+    <t>gadżety</t>
+  </si>
+  <si>
+    <t>Szablon zapytania ofertowego</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +527,21 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="11">
@@ -315,7 +606,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -458,11 +749,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -504,13 +891,373 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B2:E8" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="B2:E8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Producent" dataDxfId="12"/>
+    <tableColumn id="2" name="Punkt sprzedaży" dataDxfId="11"/>
+    <tableColumn id="3" name="PN-PT" dataDxfId="10"/>
+    <tableColumn id="4" name="SO" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:G7" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="B2:G7"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Producent" dataDxfId="7"/>
+    <tableColumn id="2" name="Przedstawiciel" dataDxfId="6"/>
+    <tableColumn id="3" name="Adres" dataDxfId="5"/>
+    <tableColumn id="4" name="Pn-Pt" dataDxfId="4"/>
+    <tableColumn id="5" name="So" dataDxfId="3"/>
+    <tableColumn id="6" name="kontakt" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -800,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J43" sqref="C40:J43"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2141,26 +2888,652 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="23"/>
+    <col min="2" max="2" width="17.85546875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="21" style="23" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="23"/>
+    <col min="7" max="7" width="11" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="23"/>
+    <col min="9" max="9" width="10" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="38.25">
+      <c r="B3" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="38.25">
+      <c r="B4" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="25.5">
+      <c r="B5" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="38.25">
+      <c r="B6" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="63.75">
+      <c r="B7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="38">
+        <v>0.6</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="38">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="38">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="38">
+        <v>7</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="38">
+        <v>7</v>
+      </c>
+      <c r="F15" s="38"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="38"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="38">
+        <v>2</v>
+      </c>
+      <c r="E17" s="38">
+        <v>3</v>
+      </c>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38">
+        <v>7</v>
+      </c>
+      <c r="F20" s="38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B22" s="24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="25.5">
+      <c r="B25" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="44"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="44" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="25.5">
+      <c r="B33" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="25.5">
+      <c r="B37" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="13.5" thickBot="1">
+      <c r="B38" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="B2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="39">
+        <v>534634300</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="23"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="39">
+        <v>601889443</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sy przedstawicieli okien dachowych
</commit_message>
<xml_diff>
--- a/plan/Zestawienie okien.xlsx
+++ b/plan/Zestawienie okien.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Zestawienie okien" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="176">
   <si>
     <t>Parter:</t>
   </si>
@@ -496,13 +496,70 @@
   </si>
   <si>
     <t>Szablon zapytania ofertowego</t>
+  </si>
+  <si>
+    <t>Roto</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>tel</t>
+  </si>
+  <si>
+    <t>Baudom</t>
+  </si>
+  <si>
+    <t>ul. Karmelkowa 29</t>
+  </si>
+  <si>
+    <t>10.00 - 18.00</t>
+  </si>
+  <si>
+    <t>10:00 - 14:00</t>
+  </si>
+  <si>
+    <t>mają Vetrex, Wiśniowski, Normstahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MADAR PREIS S.A. </t>
+  </si>
+  <si>
+    <t>ul. Kwidzyńska</t>
+  </si>
+  <si>
+    <t>Sławomir Pieniak</t>
+  </si>
+  <si>
+    <t>Manex Sp. z o.o</t>
+  </si>
+  <si>
+    <t>ul. Bystrzycka 26,</t>
+  </si>
+  <si>
+    <t>8:00-13:00</t>
+  </si>
+  <si>
+    <t>Cebj hurtonia budowlana</t>
+  </si>
+  <si>
+    <t>ul.Kłodzka 9 (Bielany)</t>
+  </si>
+  <si>
+    <t>7:00-17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:00-13:00 </t>
+  </si>
+  <si>
+    <t>uwagi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +599,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF005CA1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -849,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -924,6 +990,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1040,33 +1108,6 @@
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1206,13 +1247,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1227,34 +1261,85 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B2:E8" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B2:E8" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="B2:E8"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Producent" dataDxfId="12"/>
-    <tableColumn id="2" name="Punkt sprzedaży" dataDxfId="11"/>
-    <tableColumn id="3" name="PN-PT" dataDxfId="10"/>
-    <tableColumn id="4" name="SO" dataDxfId="9"/>
+    <tableColumn id="1" name="Producent" dataDxfId="11"/>
+    <tableColumn id="2" name="Punkt sprzedaży" dataDxfId="10"/>
+    <tableColumn id="3" name="PN-PT" dataDxfId="9"/>
+    <tableColumn id="4" name="SO" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:G7" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="B2:G7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B2:G7"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Producent" dataDxfId="7"/>
-    <tableColumn id="2" name="Przedstawiciel" dataDxfId="6"/>
-    <tableColumn id="3" name="Adres" dataDxfId="5"/>
-    <tableColumn id="4" name="Pn-Pt" dataDxfId="4"/>
-    <tableColumn id="5" name="So" dataDxfId="3"/>
-    <tableColumn id="6" name="kontakt" dataDxfId="2"/>
+    <tableColumn id="1" name="Producent" dataDxfId="5"/>
+    <tableColumn id="2" name="Przedstawiciel" dataDxfId="4"/>
+    <tableColumn id="3" name="Adres" dataDxfId="3"/>
+    <tableColumn id="4" name="Pn-Pt" dataDxfId="2"/>
+    <tableColumn id="5" name="So" dataDxfId="1"/>
+    <tableColumn id="6" name="kontakt" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B4:I13" totalsRowShown="0">
+  <autoFilter ref="B4:I13"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Producent"/>
+    <tableColumn id="2" name="Przedstawiciel"/>
+    <tableColumn id="3" name="Adres"/>
+    <tableColumn id="4" name="Pn-Pt"/>
+    <tableColumn id="5" name="So"/>
+    <tableColumn id="6" name="mail"/>
+    <tableColumn id="7" name="tel"/>
+    <tableColumn id="8" name="uwagi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2890,7 +2975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2986,7 +3071,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="63.75">
+    <row r="7" spans="2:6" ht="38.25">
       <c r="B7" s="29" t="s">
         <v>77</v>
       </c>
@@ -3437,7 +3522,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3515,25 +3600,192 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:B5"/>
+  <dimension ref="B4:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="B3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="C6" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6">
+        <v>48505508110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="C7" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" t="s">
         <v>132</v>
       </c>
+      <c r="C9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="C10" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10">
+        <v>48505508110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="C11" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="C12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F13" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wycena okien Vetrex i Oknoplast
</commit_message>
<xml_diff>
--- a/plan/Zestawienie okien.xlsx
+++ b/plan/Zestawienie okien.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Zestawienie okien" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="232">
   <si>
     <t>Parter:</t>
   </si>
@@ -531,9 +531,6 @@
     <t>szt.</t>
   </si>
   <si>
-    <t>Aprobatę techniczna InstytutuTechniki Budowlanej.</t>
-  </si>
-  <si>
     <t>Drzwi przesuwne</t>
   </si>
   <si>
@@ -677,6 +674,54 @@
   </si>
   <si>
     <t>W+R+RU</t>
+  </si>
+  <si>
+    <t>Wspolczynnik przenikalnosci swiatla</t>
+  </si>
+  <si>
+    <t>68-72</t>
+  </si>
+  <si>
+    <t>OKNOPLAST</t>
+  </si>
+  <si>
+    <t>Montaż</t>
+  </si>
+  <si>
+    <t>W+RU+U</t>
+  </si>
+  <si>
+    <t>Razem podstawowa wersja</t>
+  </si>
+  <si>
+    <t>VETREX</t>
+  </si>
+  <si>
+    <t>Dopłaty</t>
+  </si>
+  <si>
+    <t>Okno 900x1200 jako RU</t>
+  </si>
+  <si>
+    <t>Drzwi PSK</t>
+  </si>
+  <si>
+    <t>Drzwi HST</t>
+  </si>
+  <si>
+    <t>Ciepły montaż</t>
+  </si>
+  <si>
+    <t>Ciepłe parapety</t>
+  </si>
+  <si>
+    <t>Okno 1200x60 jako U</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>Rozmiar</t>
   </si>
 </sst>
 </file>
@@ -796,7 +841,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1132,11 +1177,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1243,6 +1299,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1883,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1905,19 +1987,19 @@
         <v>167</v>
       </c>
       <c r="C1" s="61" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E1" s="61" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="61" t="s">
-        <v>211</v>
-      </c>
       <c r="G1" s="61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K1" s="13"/>
       <c r="L1" s="14" t="s">
@@ -1941,7 +2023,7 @@
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="59">
         <v>1</v>
@@ -1953,10 +2035,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G2" s="2"/>
       <c r="K2" s="16"/>
@@ -1985,7 +2067,7 @@
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" s="59">
         <v>1</v>
@@ -1997,7 +2079,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3" s="59"/>
       <c r="G3" s="2"/>
@@ -2039,7 +2121,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="59"/>
       <c r="G4" s="2"/>
@@ -2075,7 +2157,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F5" s="59"/>
       <c r="G5" s="2"/>
@@ -2110,16 +2192,16 @@
       </c>
       <c r="C6" s="60"/>
       <c r="D6" s="59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="F6" s="59" t="s">
-        <v>214</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K6" s="16"/>
       <c r="L6" s="3" t="s">
@@ -2143,7 +2225,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" s="59">
         <v>1</v>
@@ -2155,10 +2237,10 @@
         <v>1</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G7" s="2"/>
       <c r="K7" s="16"/>
@@ -2207,7 +2289,7 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8" s="59">
         <v>1</v>
@@ -2219,7 +2301,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F8" s="59"/>
       <c r="G8" s="2"/>
@@ -2295,10 +2377,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1"/>
@@ -2377,10 +2459,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G10" s="2"/>
       <c r="K10" s="16" t="s">
@@ -2458,10 +2540,10 @@
         <v>10</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G11" s="2"/>
       <c r="K11" s="16" t="s">
@@ -2577,7 +2659,7 @@
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B14" s="59">
         <v>2</v>
@@ -2589,7 +2671,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F14" s="59"/>
       <c r="G14" s="2"/>
@@ -2623,7 +2705,7 @@
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B15" s="59">
         <v>2</v>
@@ -2655,7 +2737,7 @@
     </row>
     <row r="16" spans="1:27">
       <c r="A16" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16" s="59">
         <v>2</v>
@@ -2667,7 +2749,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F16" s="59"/>
       <c r="G16" s="2"/>
@@ -2761,7 +2843,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F18" s="59"/>
       <c r="G18" s="2"/>
@@ -2842,10 +2924,10 @@
         <v>1</v>
       </c>
       <c r="E19" s="59" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G19" s="2"/>
       <c r="K19" s="16" t="s">
@@ -3090,7 +3172,7 @@
     </row>
     <row r="23" spans="1:28">
       <c r="A23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K23" s="16"/>
       <c r="L23" s="2"/>
@@ -3125,7 +3207,7 @@
     </row>
     <row r="24" spans="1:28">
       <c r="A24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K24" s="16"/>
       <c r="L24" s="2"/>
@@ -3155,7 +3237,7 @@
     </row>
     <row r="25" spans="1:28">
       <c r="A25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K25" s="16"/>
       <c r="L25" s="2"/>
@@ -3187,7 +3269,7 @@
     </row>
     <row r="26" spans="1:28">
       <c r="A26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K26" s="16"/>
       <c r="L26" s="2"/>
@@ -3209,7 +3291,7 @@
     </row>
     <row r="27" spans="1:28">
       <c r="A27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="2" t="s">
@@ -3274,10 +3356,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G40"/>
+  <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3288,13 +3370,16 @@
     <col min="4" max="4" width="19.42578125" style="22" customWidth="1"/>
     <col min="5" max="5" width="25.140625" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="22"/>
-    <col min="9" max="9" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="22"/>
+    <col min="7" max="8" width="15.140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="22" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="22"/>
+    <col min="13" max="13" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" style="22" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="2:16">
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24" t="s">
@@ -3302,7 +3387,7 @@
       </c>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:16" ht="15.75" thickBot="1">
       <c r="B2" s="31" t="s">
         <v>57</v>
       </c>
@@ -3315,8 +3400,28 @@
       <c r="E2" s="33" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="38.25">
+      <c r="I2" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="63" t="s">
+        <v>231</v>
+      </c>
+      <c r="L2" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="M2" s="63" t="s">
+        <v>218</v>
+      </c>
+      <c r="N2" s="63" t="s">
+        <v>222</v>
+      </c>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+    </row>
+    <row r="3" spans="2:16" ht="39">
       <c r="B3" s="28" t="s">
         <v>58</v>
       </c>
@@ -3329,8 +3434,26 @@
       <c r="E3" s="29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="38.25">
+      <c r="I3" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" s="64">
+        <v>1</v>
+      </c>
+      <c r="K3" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="64" t="s">
+        <v>211</v>
+      </c>
+      <c r="M3" s="64">
+        <v>500.11</v>
+      </c>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="2:16" ht="39">
       <c r="B4" s="28" t="s">
         <v>58</v>
       </c>
@@ -3343,8 +3466,26 @@
       <c r="E4" s="29" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="25.5">
+      <c r="I4" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" s="59">
+        <v>1</v>
+      </c>
+      <c r="K4" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="M4" s="59">
+        <v>702.82</v>
+      </c>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="2:16" ht="26.25">
       <c r="B5" s="28" t="s">
         <v>58</v>
       </c>
@@ -3357,8 +3498,26 @@
       <c r="E5" s="30" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="38.25">
+      <c r="I5" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="59">
+        <v>2</v>
+      </c>
+      <c r="K5" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="M5" s="59">
+        <v>1203.07</v>
+      </c>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="17"/>
+    </row>
+    <row r="6" spans="2:16" ht="39">
       <c r="B6" s="28" t="s">
         <v>65</v>
       </c>
@@ -3371,8 +3530,26 @@
       <c r="E6" s="29" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="38.25">
+      <c r="I6" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="59">
+        <v>1</v>
+      </c>
+      <c r="K6" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="M6" s="59">
+        <v>1526.35</v>
+      </c>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16" ht="39">
       <c r="B7" s="28" t="s">
         <v>66</v>
       </c>
@@ -3385,8 +3562,26 @@
       <c r="E7" s="29" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="I7" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="59">
+        <v>3</v>
+      </c>
+      <c r="K7" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="L7" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="M7" s="59">
+        <v>3861.89</v>
+      </c>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="17"/>
+    </row>
+    <row r="8" spans="2:16" ht="15">
       <c r="B8" s="34" t="s">
         <v>67</v>
       </c>
@@ -3397,13 +3592,89 @@
       <c r="E8" s="36" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="I8" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J8" s="59">
+        <v>1</v>
+      </c>
+      <c r="K8" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="M8" s="59">
+        <v>500.11</v>
+      </c>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="2:16" ht="15">
+      <c r="I9" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="J9" s="59">
+        <v>1</v>
+      </c>
+      <c r="K9" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="M9" s="59">
+        <v>1040.4100000000001</v>
+      </c>
+      <c r="N9" s="59"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="2:16" ht="15">
+      <c r="I10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="59">
+        <v>1</v>
+      </c>
+      <c r="K10" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="M10" s="59">
+        <v>372.23</v>
+      </c>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="17"/>
+    </row>
+    <row r="11" spans="2:16" ht="15">
       <c r="B11" s="23" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="I11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="59">
+        <v>1</v>
+      </c>
+      <c r="K11" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="M11" s="59">
+        <v>372.23</v>
+      </c>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="17"/>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" thickBot="1">
       <c r="B12" s="24" t="s">
         <v>57</v>
       </c>
@@ -3419,8 +3690,26 @@
       <c r="F12" s="25" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="2:6">
+      <c r="I12" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="65">
+        <v>1</v>
+      </c>
+      <c r="K12" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="M12" s="65">
+        <v>372.23</v>
+      </c>
+      <c r="N12" s="65"/>
+      <c r="O12" s="65"/>
+      <c r="P12" s="20"/>
+    </row>
+    <row r="13" spans="2:16" ht="15.75" thickBot="1">
       <c r="B13" s="25" t="s">
         <v>104</v>
       </c>
@@ -3436,8 +3725,16 @@
       <c r="F13" s="37" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="I13" s="66"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="67"/>
+      <c r="P13" s="66"/>
+    </row>
+    <row r="14" spans="2:16" ht="15">
       <c r="B14" s="25" t="s">
         <v>70</v>
       </c>
@@ -3453,8 +3750,18 @@
       <c r="F14" s="37">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="I14" s="68" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="15"/>
+    </row>
+    <row r="15" spans="2:16" ht="15">
       <c r="B15" s="25" t="s">
         <v>105</v>
       </c>
@@ -3468,8 +3775,26 @@
         <v>7</v>
       </c>
       <c r="F15" s="37"/>
-    </row>
-    <row r="16" spans="2:6">
+      <c r="I15" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="J15" s="59">
+        <v>2</v>
+      </c>
+      <c r="K15" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="M15" s="59">
+        <v>2152.1</v>
+      </c>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="17"/>
+    </row>
+    <row r="16" spans="2:16" ht="15">
       <c r="B16" s="25" t="s">
         <v>106</v>
       </c>
@@ -3483,8 +3808,26 @@
         <v>71</v>
       </c>
       <c r="F16" s="37"/>
-    </row>
-    <row r="17" spans="2:7">
+      <c r="I16" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="J16" s="59">
+        <v>2</v>
+      </c>
+      <c r="K16" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="M16" s="59">
+        <v>2152.1</v>
+      </c>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="2:16" ht="15">
       <c r="B17" s="25" t="s">
         <v>107</v>
       </c>
@@ -3498,8 +3841,26 @@
         <v>3</v>
       </c>
       <c r="F17" s="37"/>
-    </row>
-    <row r="18" spans="2:7">
+      <c r="I17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="59">
+        <v>1</v>
+      </c>
+      <c r="K17" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="M17" s="59">
+        <v>445.56</v>
+      </c>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="17"/>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" thickBot="1">
       <c r="B18" s="25" t="s">
         <v>108</v>
       </c>
@@ -3513,8 +3874,26 @@
         <v>78</v>
       </c>
       <c r="F18" s="37"/>
-    </row>
-    <row r="19" spans="2:7">
+      <c r="I18" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="65">
+        <v>1</v>
+      </c>
+      <c r="K18" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="65" t="s">
+        <v>211</v>
+      </c>
+      <c r="M18" s="65">
+        <v>500.11</v>
+      </c>
+      <c r="N18" s="65"/>
+      <c r="O18" s="65"/>
+      <c r="P18" s="20"/>
+    </row>
+    <row r="19" spans="2:16" ht="15.75" thickBot="1">
       <c r="B19" s="25" t="s">
         <v>109</v>
       </c>
@@ -3524,8 +3903,16 @@
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="37"/>
-    </row>
-    <row r="20" spans="2:7">
+      <c r="I19" s="66"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="66"/>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" thickBot="1">
       <c r="B20" s="25" t="s">
         <v>110</v>
       </c>
@@ -3537,13 +3924,53 @@
       <c r="F20" s="37">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="13.5" thickBot="1">
+      <c r="I20" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="J20" s="70"/>
+      <c r="K20" s="70"/>
+      <c r="L20" s="70"/>
+      <c r="M20" s="70">
+        <v>2230.8000000000002</v>
+      </c>
+      <c r="N20" s="70">
+        <v>1692</v>
+      </c>
+      <c r="O20" s="70"/>
+      <c r="P20" s="71"/>
+    </row>
+    <row r="21" spans="2:16" ht="13.5" thickBot="1">
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="72"/>
+      <c r="O21" s="72"/>
+      <c r="P21" s="72"/>
+    </row>
+    <row r="22" spans="2:16" ht="13.5" thickBot="1">
       <c r="B22" s="23" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="13.5" thickBot="1">
+      <c r="I22" s="77" t="s">
+        <v>221</v>
+      </c>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="73">
+        <f>SUM(M3:M20)</f>
+        <v>17932.12</v>
+      </c>
+      <c r="N22" s="73">
+        <f>13561+N20</f>
+        <v>15253</v>
+      </c>
+      <c r="O22" s="53"/>
+      <c r="P22" s="54"/>
+    </row>
+    <row r="23" spans="2:16" ht="13.5" thickBot="1">
       <c r="B23" s="55" t="s">
         <v>104</v>
       </c>
@@ -3551,15 +3978,24 @@
         <v>137</v>
       </c>
       <c r="D23" s="51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E23" s="53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="54"/>
-    </row>
-    <row r="24" spans="2:7">
+      <c r="H23" s="62"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="72"/>
+    </row>
+    <row r="24" spans="2:16">
       <c r="B24" s="56" t="s">
         <v>70</v>
       </c>
@@ -3574,8 +4010,19 @@
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="50"/>
-    </row>
-    <row r="25" spans="2:7" ht="25.5">
+      <c r="H24" s="62"/>
+      <c r="I24" s="76" t="s">
+        <v>223</v>
+      </c>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="74"/>
+      <c r="P24" s="75"/>
+    </row>
+    <row r="25" spans="2:16" ht="25.5">
       <c r="B25" s="57" t="s">
         <v>105</v>
       </c>
@@ -3583,15 +4030,30 @@
         <v>127</v>
       </c>
       <c r="D25" s="57" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25" s="45"/>
-    </row>
-    <row r="26" spans="2:7">
+      <c r="H25" s="62"/>
+      <c r="I25" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24">
+        <v>202.71</v>
+      </c>
+      <c r="N25" s="24">
+        <v>259</v>
+      </c>
+      <c r="O25" s="24"/>
+      <c r="P25" s="45"/>
+    </row>
+    <row r="26" spans="2:16">
       <c r="B26" s="57" t="s">
         <v>107</v>
       </c>
@@ -3599,15 +4061,30 @@
         <v>138</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F26" s="24"/>
       <c r="G26" s="45"/>
-    </row>
-    <row r="27" spans="2:7">
+      <c r="H26" s="62"/>
+      <c r="I26" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24">
+        <v>153.9</v>
+      </c>
+      <c r="N26" s="24">
+        <v>215</v>
+      </c>
+      <c r="O26" s="24"/>
+      <c r="P26" s="45"/>
+    </row>
+    <row r="27" spans="2:16">
       <c r="B27" s="57" t="s">
         <v>106</v>
       </c>
@@ -3615,43 +4092,88 @@
         <v>131</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F27" s="24"/>
       <c r="G27" s="45"/>
-    </row>
-    <row r="28" spans="2:7">
+      <c r="H27" s="62"/>
+      <c r="I27" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24">
+        <v>2271.15</v>
+      </c>
+      <c r="N27" s="24">
+        <v>1295</v>
+      </c>
+      <c r="O27" s="24"/>
+      <c r="P27" s="45"/>
+    </row>
+    <row r="28" spans="2:16">
       <c r="B28" s="57" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" s="43"/>
       <c r="D28" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F28" s="24"/>
       <c r="G28" s="45"/>
-    </row>
-    <row r="29" spans="2:7">
+      <c r="H28" s="62"/>
+      <c r="I28" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24">
+        <v>7025.04</v>
+      </c>
+      <c r="N28" s="24">
+        <v>10869</v>
+      </c>
+      <c r="O28" s="24"/>
+      <c r="P28" s="45"/>
+    </row>
+    <row r="29" spans="2:16">
       <c r="B29" s="57" t="s">
         <v>108</v>
       </c>
       <c r="C29" s="43"/>
       <c r="D29" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F29" s="24"/>
       <c r="G29" s="45"/>
-    </row>
-    <row r="30" spans="2:7">
+      <c r="H29" s="62"/>
+      <c r="I29" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="N29" s="24">
+        <v>2956</v>
+      </c>
+      <c r="O29" s="24"/>
+      <c r="P29" s="45"/>
+    </row>
+    <row r="30" spans="2:16" ht="13.5" thickBot="1">
       <c r="B30" s="57" t="s">
         <v>110</v>
       </c>
@@ -3659,15 +4181,30 @@
         <v>134</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F30" s="24"/>
       <c r="G30" s="45"/>
-    </row>
-    <row r="31" spans="2:7">
+      <c r="H30" s="62"/>
+      <c r="I30" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="N30" s="46">
+        <v>274</v>
+      </c>
+      <c r="O30" s="46"/>
+      <c r="P30" s="47"/>
+    </row>
+    <row r="31" spans="2:16">
       <c r="B31" s="57" t="s">
         <v>123</v>
       </c>
@@ -3675,15 +4212,16 @@
         <v>139</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F31" s="24"/>
       <c r="G31" s="45"/>
-    </row>
-    <row r="32" spans="2:7">
+      <c r="H31" s="62"/>
+    </row>
+    <row r="32" spans="2:16">
       <c r="B32" s="57" t="s">
         <v>124</v>
       </c>
@@ -3691,15 +4229,16 @@
         <v>139</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F32" s="24"/>
       <c r="G32" s="45"/>
-    </row>
-    <row r="33" spans="2:7">
+      <c r="H32" s="62"/>
+    </row>
+    <row r="33" spans="2:8">
       <c r="B33" s="57" t="s">
         <v>125</v>
       </c>
@@ -3707,31 +4246,33 @@
         <v>140</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F33" s="24"/>
       <c r="G33" s="45"/>
-    </row>
-    <row r="34" spans="2:7">
+      <c r="H33" s="62"/>
+    </row>
+    <row r="34" spans="2:8">
       <c r="B34" s="57" t="s">
+        <v>168</v>
+      </c>
+      <c r="C34" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="C34" s="43" t="s">
-        <v>170</v>
-      </c>
       <c r="D34" s="39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F34" s="24"/>
       <c r="G34" s="45"/>
-    </row>
-    <row r="35" spans="2:7" ht="25.5">
+      <c r="H34" s="62"/>
+    </row>
+    <row r="35" spans="2:8" ht="25.5">
       <c r="B35" s="57" t="s">
         <v>126</v>
       </c>
@@ -3739,15 +4280,16 @@
         <v>128</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F35" s="24"/>
       <c r="G35" s="45"/>
-    </row>
-    <row r="36" spans="2:7">
+      <c r="H35" s="62"/>
+    </row>
+    <row r="36" spans="2:8">
       <c r="B36" s="57" t="s">
         <v>129</v>
       </c>
@@ -3755,15 +4297,16 @@
         <v>130</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="45"/>
-    </row>
-    <row r="37" spans="2:7">
+      <c r="H36" s="62"/>
+    </row>
+    <row r="37" spans="2:8">
       <c r="B37" s="57" t="s">
         <v>132</v>
       </c>
@@ -3771,27 +4314,31 @@
         <v>136</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="45"/>
-    </row>
-    <row r="38" spans="2:7" ht="28.5" customHeight="1">
+      <c r="H37" s="62"/>
+    </row>
+    <row r="38" spans="2:8" ht="28.5" customHeight="1">
       <c r="B38" s="57" t="s">
-        <v>168</v>
+        <v>216</v>
       </c>
       <c r="C38" s="43" t="s">
         <v>133</v>
       </c>
       <c r="D38" s="39"/>
-      <c r="E38" s="24"/>
+      <c r="E38" s="24" t="s">
+        <v>217</v>
+      </c>
       <c r="F38" s="24"/>
       <c r="G38" s="45"/>
-    </row>
-    <row r="39" spans="2:7" ht="25.5">
+      <c r="H38" s="62"/>
+    </row>
+    <row r="39" spans="2:8" ht="25.5">
       <c r="B39" s="57" t="s">
         <v>135</v>
       </c>
@@ -3802,8 +4349,9 @@
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
       <c r="G39" s="45"/>
-    </row>
-    <row r="40" spans="2:7" ht="13.5" thickBot="1">
+      <c r="H39" s="62"/>
+    </row>
+    <row r="40" spans="2:8" ht="13.5" thickBot="1">
       <c r="B40" s="58" t="s">
         <v>142</v>
       </c>
@@ -3814,6 +4362,7 @@
       <c r="E40" s="46"/>
       <c r="F40" s="46"/>
       <c r="G40" s="47"/>
+      <c r="H40" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>